<commit_message>
Cost column added to dummy xlsx
</commit_message>
<xml_diff>
--- a/inst/docs/dummyPortfolio.xlsx
+++ b/inst/docs/dummyPortfolio.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardo/Dropbox (Personal)/Documentos/R/Github/lares/inst/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D749372-A431-F149-8681-2AB0F1664BE1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0636520-BB77-F145-881B-4486E2D52756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9740" yWindow="460" windowWidth="19060" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portafolio" sheetId="5" r:id="rId1"/>
     <sheet name="Fondos" sheetId="2" r:id="rId2"/>
     <sheet name="Transacciones" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>US Stocks</t>
   </si>
@@ -141,6 +147,9 @@
   </si>
   <si>
     <t>Travel payment</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -204,6 +213,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -211,6 +221,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -841,7 +852,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -971,26 +1042,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1053,16 +1104,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -1161,16 +1202,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1185,29 +1216,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="36">
   <sortState ref="A2:H12">
     <sortCondition descending="1" ref="C2"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stocks" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stocks" dataDxfId="34">
       <calculatedColumnFormula>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Quant])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Invested" dataDxfId="30" dataCellStyle="Moneda [0]">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Invested" dataDxfId="33" dataCellStyle="Moneda [0]">
       <calculatedColumnFormula>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="StockIniValue" dataDxfId="29">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="StockIniValue" dataDxfId="32">
       <calculatedColumnFormula>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="InvPerc" dataDxfId="28" dataCellStyle="Porcentaje">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="InvPerc" dataDxfId="31" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Trans" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Trans" dataDxfId="30">
       <calculatedColumnFormula>COUNTIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ABF5D390-FC0A-CD4D-9AA4-B3BA2EA3CC23}" name="StartDate" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{ABF5D390-FC0A-CD4D-9AA4-B3BA2EA3CC23}" name="StartDate" dataDxfId="29">
       <calculatedColumnFormula>VLOOKUP(Tabla2[[#This Row],[Symbol]]&amp;"1",Tabla1[[CODE]:[Date]],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1216,39 +1247,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla3" displayName="Tabla3" ref="A1:D8" totalsRowShown="0" dataDxfId="24" dataCellStyle="Moneda [0]">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla3" displayName="Tabla3" ref="A1:D8" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda [0]">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="27">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cash" dataDxfId="21" dataCellStyle="Moneda [0]"/>
-    <tableColumn id="4" xr3:uid="{1CA1CDD9-23E9-5C43-B7F2-56E6F032861A}" name="Concepto" dataDxfId="20" dataCellStyle="Moneda [0]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cash" dataDxfId="25" dataCellStyle="Moneda [0]"/>
+    <tableColumn id="4" xr3:uid="{1CA1CDD9-23E9-5C43-B7F2-56E6F032861A}" name="Concepto" dataDxfId="24" dataCellStyle="Moneda [0]"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla1" displayName="Tabla1" ref="A1:I18" totalsRowShown="0">
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla1" displayName="Tabla1" ref="A1:J18" totalsRowShown="0">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Inv" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Inv" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>COUNTIF(D$2:D2,Tabla1[[#This Row],[Symbol]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{04CD5116-8E90-834C-BF7D-8FB44C956722}" name="CODE" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="10" xr3:uid="{04CD5116-8E90-834C-BF7D-8FB44C956722}" name="CODE" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula>Tabla1[[#This Row],[Symbol]]&amp;Tabla1[[#This Row],[Inv]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Symbol" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Date" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Quant" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Value" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Amount" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Symbol" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Date" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Quant" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Value" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{45F45114-913F-274A-B327-91BFC2BFF766}" name="Cost" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Amount" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Description" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Description" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1521,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1918,7 +1950,7 @@
     <sortCondition descending="1" ref="C2"/>
   </sortState>
   <conditionalFormatting sqref="H2:H12">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2063,7 +2095,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2077,11 +2109,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2091,12 +2121,12 @@
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="7" customWidth="1"/>
+    <col min="7" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
@@ -2118,14 +2148,17 @@
       <c r="G1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -2151,15 +2184,18 @@
         <v>57</v>
       </c>
       <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>2857</v>
       </c>
-      <c r="I2" s="2" t="str">
+      <c r="J2" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>50 @57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A11" si="0">ROW()-1</f>
         <v>2</v>
@@ -2185,15 +2221,18 @@
         <v>87.75</v>
       </c>
       <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>2639.5</v>
       </c>
-      <c r="I3" s="2" t="str">
+      <c r="J3" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>30 @87,75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2219,15 +2258,18 @@
         <v>84</v>
       </c>
       <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>2527</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="J4" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>30 @84</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2253,15 +2295,18 @@
         <v>135.38</v>
       </c>
       <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>10837.4</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="J5" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>80 @135,38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2287,15 +2332,18 @@
         <v>65.739999999999995</v>
       </c>
       <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>3293.9999999999995</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="J6" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>50 @65,74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2321,15 +2369,18 @@
         <v>56.4</v>
       </c>
       <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1699</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="J7" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>30 @56,4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2355,15 +2406,18 @@
         <v>37</v>
       </c>
       <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>3707</v>
       </c>
-      <c r="I8" s="2" t="str">
+      <c r="J8" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>100 @37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2389,15 +2443,18 @@
         <v>35.85</v>
       </c>
       <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1799.5</v>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="J9" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>50 @35,85</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2423,15 +2480,18 @@
         <v>1027.8</v>
       </c>
       <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>10285</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="J10" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>10 @1027,8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2457,15 +2517,18 @@
         <v>137.65</v>
       </c>
       <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>2071.75</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="J11" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>15 @137,65</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f>ROW()-1</f>
         <v>11</v>
@@ -2492,15 +2555,18 @@
         <v>144.44999999999999</v>
       </c>
       <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>5785</v>
       </c>
-      <c r="I12" s="20" t="str">
+      <c r="J12" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>40 @144,45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f>ROW()-1</f>
         <v>12</v>
@@ -2526,15 +2592,18 @@
         <v>135.34</v>
       </c>
       <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1360.4</v>
       </c>
-      <c r="I13" s="20" t="str">
+      <c r="J13" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>10 @135,34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" ref="A14:A18" si="1">ROW()-1</f>
         <v>13</v>
@@ -2560,15 +2629,18 @@
         <v>55.49</v>
       </c>
       <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1671.7</v>
       </c>
-      <c r="I14" s="20" t="str">
+      <c r="J14" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>30 @55,49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2594,15 +2666,18 @@
         <v>65.28</v>
       </c>
       <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1312.6</v>
       </c>
-      <c r="I15" s="20" t="str">
+      <c r="J15" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>20 @65,28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2628,15 +2703,18 @@
         <v>277.5</v>
       </c>
       <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>2782</v>
       </c>
-      <c r="I16" s="20" t="str">
+      <c r="J16" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>10 @277,5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2662,15 +2740,18 @@
         <v>33.299999999999997</v>
       </c>
       <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>1671.9999999999998</v>
       </c>
-      <c r="I17" s="20" t="str">
+      <c r="J17" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>50 @33,3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -2696,10 +2777,13 @@
         <v>261</v>
       </c>
       <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
         <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
         <v>5227</v>
       </c>
-      <c r="I18" s="20" t="str">
+      <c r="J18" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
         <v>20 @261</v>
       </c>
@@ -2709,12 +2793,12 @@
     <sortCondition ref="E2"/>
   </sortState>
   <conditionalFormatting sqref="E2:E5">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Readme update + xlsx file fix
</commit_message>
<xml_diff>
--- a/inst/docs/dummyPortfolio.xlsx
+++ b/inst/docs/dummyPortfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardo/Dropbox (Personal)/Documentos/R/Github/lares/inst/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardolares/Dropbox (Personal)/Documentos/R/Github/lares/inst/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0636520-BB77-F145-881B-4486E2D52756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCEE8CC-AB0E-EF47-9191-91A2602D3FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="460" windowWidth="19060" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9740" yWindow="460" windowWidth="19060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portafolio" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -157,11 +159,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -258,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -528,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -541,11 +543,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -563,7 +565,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -571,290 +573,290 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="266">
-    <cellStyle name="Hipervínculo" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="196" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="212" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="228" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="244" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="250" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="234" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="218" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="202" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="190" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="256" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="260" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="264" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="262" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="258" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="194" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="210" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="226" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="242" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="252" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="236" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="220" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="204" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="188" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="232" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="216" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="208" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="200" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="192" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="224" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="230" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="238" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="246" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="248" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="240" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="254" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="214" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="222" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="206" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="198" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="251" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="257" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="261" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="263" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="265" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="259" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="249" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="253" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="255" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Moneda [0]" xfId="3" builtinId="7"/>
+    <cellStyle name="Currency [0]" xfId="3" builtinId="7"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="4" builtinId="5"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="37">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -864,7 +866,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -874,55 +884,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -932,7 +894,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -942,7 +904,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -952,7 +914,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -968,7 +930,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -978,7 +940,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1042,20 +1004,23 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FF006100"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1073,20 +1038,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1104,9 +1055,50 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+      <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1138,7 +1130,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1156,7 +1148,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1202,6 +1194,16 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1216,29 +1218,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="36">
-  <sortState ref="A2:H12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
     <sortCondition descending="1" ref="C2"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stocks" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stocks" dataDxfId="33">
       <calculatedColumnFormula>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Quant])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Invested" dataDxfId="33" dataCellStyle="Moneda [0]">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Invested" dataDxfId="32">
       <calculatedColumnFormula>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="StockIniValue" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="StockIniValue" dataDxfId="31">
       <calculatedColumnFormula>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="InvPerc" dataDxfId="31" dataCellStyle="Porcentaje">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="InvPerc" dataDxfId="30">
       <calculatedColumnFormula>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Trans" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Trans" dataDxfId="29">
       <calculatedColumnFormula>COUNTIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ABF5D390-FC0A-CD4D-9AA4-B3BA2EA3CC23}" name="StartDate" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{ABF5D390-FC0A-CD4D-9AA4-B3BA2EA3CC23}" name="StartDate" dataDxfId="28">
       <calculatedColumnFormula>VLOOKUP(Tabla2[[#This Row],[Symbol]]&amp;"1",Tabla1[[CODE]:[Date]],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1247,14 +1249,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla3" displayName="Tabla3" ref="A1:D8" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda [0]">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla3" displayName="Tabla3" ref="A1:D8" totalsRowShown="0" dataDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="25">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cash" dataDxfId="25" dataCellStyle="Moneda [0]"/>
-    <tableColumn id="4" xr3:uid="{1CA1CDD9-23E9-5C43-B7F2-56E6F032861A}" name="Concepto" dataDxfId="24" dataCellStyle="Moneda [0]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cash" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{1CA1CDD9-23E9-5C43-B7F2-56E6F032861A}" name="Concepto" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1263,24 +1265,24 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla1" displayName="Tabla1" ref="A1:J18" totalsRowShown="0">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Inv" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Inv" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula>COUNTIF(D$2:D2,Tabla1[[#This Row],[Symbol]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{04CD5116-8E90-834C-BF7D-8FB44C956722}" name="CODE" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="10" xr3:uid="{04CD5116-8E90-834C-BF7D-8FB44C956722}" name="CODE" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>Tabla1[[#This Row],[Symbol]]&amp;Tabla1[[#This Row],[Inv]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Symbol" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Date" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Quant" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Value" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{45F45114-913F-274A-B327-91BFC2BFF766}" name="Cost" dataDxfId="0" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Amount" dataDxfId="9" totalsRowDxfId="8">
-      <calculatedColumnFormula>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Symbol" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Date" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Quant" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Value" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{45F45114-913F-274A-B327-91BFC2BFF766}" name="Cost" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Amount" dataDxfId="0" totalsRowDxfId="3">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Description" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Description" dataDxfId="2" totalsRowDxfId="1">
       <calculatedColumnFormula>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1553,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1603,15 +1605,15 @@
       </c>
       <c r="C2" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>20054.550000000003</v>
+        <v>20026.550000000003</v>
       </c>
       <c r="D2" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>138.30724137931037</v>
+        <v>138.11413793103449</v>
       </c>
       <c r="E2" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>0.32594264223437036</v>
+        <v>0.32600681916039193</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1635,15 +1637,15 @@
       </c>
       <c r="C3" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>10285</v>
+        <v>10278</v>
       </c>
       <c r="D3" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>1028.5</v>
+        <v>1027.8</v>
       </c>
       <c r="E3" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>0.16716007466537511</v>
+        <v>0.16731279662900039</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -1667,15 +1669,15 @@
       </c>
       <c r="C4" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>8009</v>
+        <v>7995</v>
       </c>
       <c r="D4" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>266.96666666666664</v>
+        <v>266.5</v>
       </c>
       <c r="E4" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>0.13016869596451039</v>
+        <v>0.13014845388683188</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -1699,15 +1701,15 @@
       </c>
       <c r="C5" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>4606.5999999999995</v>
+        <v>4592.5999999999995</v>
       </c>
       <c r="D5" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>65.808571428571426</v>
+        <v>65.608571428571423</v>
       </c>
       <c r="E5" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>7.4870160423287979E-2</v>
+        <v>7.4761699727412645E-2</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1731,15 +1733,15 @@
       </c>
       <c r="C6" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>4528.7</v>
+        <v>4521.7</v>
       </c>
       <c r="D6" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>56.608750000000001</v>
+        <v>56.521249999999995</v>
       </c>
       <c r="E6" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>7.360406710132078E-2</v>
+        <v>7.3607537703575698E-2</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
@@ -1763,15 +1765,15 @@
       </c>
       <c r="C7" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>3707</v>
+        <v>3700</v>
       </c>
       <c r="D7" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>37.07</v>
+        <v>37</v>
       </c>
       <c r="E7" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>6.0249139210942687E-2</v>
+        <v>6.0231304487964731E-2</v>
       </c>
       <c r="F7" t="s">
         <v>2</v>
@@ -1803,7 +1805,7 @@
       </c>
       <c r="E8" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>4.289927244329194E-2</v>
+        <v>4.2967710323238623E-2</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
@@ -1835,7 +1837,7 @@
       </c>
       <c r="E9" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>4.1070832151619142E-2</v>
+        <v>4.1136353092185642E-2</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -1859,15 +1861,15 @@
       </c>
       <c r="C10" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>1799.5</v>
+        <v>1792.5</v>
       </c>
       <c r="D10" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>35.99</v>
+        <v>35.85</v>
       </c>
       <c r="E10" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>2.9246918265468401E-2</v>
+        <v>2.9179625214777506E-2</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
@@ -1891,15 +1893,15 @@
       </c>
       <c r="C11" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>1699</v>
+        <v>1692</v>
       </c>
       <c r="D11" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>56.633333333333333</v>
+        <v>56.4</v>
       </c>
       <c r="E11" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>2.7613511604907371E-2</v>
+        <v>2.7543612755036844E-2</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -1923,15 +1925,15 @@
       </c>
       <c r="C12" s="9">
         <f>SUMIF(Tabla1[Symbol],Tabla2[[#This Row],[Symbol]],Tabla1[Amount])</f>
-        <v>1671.9999999999998</v>
+        <v>1664.9999999999998</v>
       </c>
       <c r="D12" s="18">
         <f>IFERROR(Tabla2[[#This Row],[Invested]]/Tabla2[[#This Row],[Stocks]],0)</f>
-        <v>33.44</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="E12" s="17">
         <f>Tabla2[[#This Row],[Invested]]/SUM(Tabla2[Invested])</f>
-        <v>2.7174685934905896E-2</v>
+        <v>2.7104087019584125E-2</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
@@ -1946,11 +1948,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
     <sortCondition descending="1" ref="C2"/>
   </sortState>
   <conditionalFormatting sqref="H2:H12">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1967,7 +1969,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,7 +2011,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A3:A8" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="8">
@@ -2024,7 +2026,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="8">
@@ -2039,6 +2041,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="8">
@@ -2053,6 +2056,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="8">
@@ -2067,6 +2071,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="8">
@@ -2081,6 +2086,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="8">
@@ -2095,7 +2101,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2111,7 +2117,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2184,10 +2192,10 @@
         <v>57</v>
       </c>
       <c r="H2" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
         <v>2857</v>
       </c>
       <c r="J2" s="2" t="str">
@@ -2221,10 +2229,10 @@
         <v>87.75</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
         <v>2639.5</v>
       </c>
       <c r="J3" s="2" t="str">
@@ -2258,10 +2266,10 @@
         <v>84</v>
       </c>
       <c r="H4" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I4" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
         <v>2527</v>
       </c>
       <c r="J4" s="2" t="str">
@@ -2298,8 +2306,8 @@
         <v>0</v>
       </c>
       <c r="I5" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>10837.4</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>10830.4</v>
       </c>
       <c r="J5" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2335,8 +2343,8 @@
         <v>0</v>
       </c>
       <c r="I6" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>3293.9999999999995</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>3286.9999999999995</v>
       </c>
       <c r="J6" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2372,8 +2380,8 @@
         <v>0</v>
       </c>
       <c r="I7" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1699</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1692</v>
       </c>
       <c r="J7" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2409,8 +2417,8 @@
         <v>0</v>
       </c>
       <c r="I8" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>3707</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>3700</v>
       </c>
       <c r="J8" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2446,8 +2454,8 @@
         <v>0</v>
       </c>
       <c r="I9" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1799.5</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1792.5</v>
       </c>
       <c r="J9" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2483,8 +2491,8 @@
         <v>0</v>
       </c>
       <c r="I10" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>10285</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>10278</v>
       </c>
       <c r="J10" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2520,8 +2528,8 @@
         <v>0</v>
       </c>
       <c r="I11" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>2071.75</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>2064.75</v>
       </c>
       <c r="J11" s="2" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2558,8 +2566,8 @@
         <v>0</v>
       </c>
       <c r="I12" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>5785</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>5778</v>
       </c>
       <c r="J12" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2572,7 +2580,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="16">
-        <f>COUNTIF(D$2:D18,Tabla1[[#This Row],[Symbol]])</f>
+        <f>COUNTIF(D$2:D13,Tabla1[[#This Row],[Symbol]])</f>
         <v>4</v>
       </c>
       <c r="C13" t="str">
@@ -2595,8 +2603,8 @@
         <v>0</v>
       </c>
       <c r="I13" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1360.4</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1353.4</v>
       </c>
       <c r="J13" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2632,8 +2640,8 @@
         <v>0</v>
       </c>
       <c r="I14" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1671.7</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1664.7</v>
       </c>
       <c r="J14" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2646,7 +2654,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="16">
-        <f>COUNTIF(D$2:D18,Tabla1[[#This Row],[Symbol]])</f>
+        <f>COUNTIF(D$2:D15,Tabla1[[#This Row],[Symbol]])</f>
         <v>2</v>
       </c>
       <c r="C15" t="str">
@@ -2669,8 +2677,8 @@
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1312.6</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1305.5999999999999</v>
       </c>
       <c r="J15" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2706,8 +2714,8 @@
         <v>0</v>
       </c>
       <c r="I16" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>2782</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>2775</v>
       </c>
       <c r="J16" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2720,7 +2728,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16">
-        <f>COUNTIF(D$2:D18,Tabla1[[#This Row],[Symbol]])</f>
+        <f>COUNTIF(D$2:D17,Tabla1[[#This Row],[Symbol]])</f>
         <v>1</v>
       </c>
       <c r="C17" t="str">
@@ -2743,8 +2751,8 @@
         <v>0</v>
       </c>
       <c r="I17" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>1671.9999999999998</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>1664.9999999999998</v>
       </c>
       <c r="J17" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2780,8 +2788,8 @@
         <v>0</v>
       </c>
       <c r="I18" s="3">
-        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+7</f>
-        <v>5227</v>
+        <f>Tabla1[[#This Row],[Value]]*Tabla1[[#This Row],[Quant]]+Tabla1[[#This Row],[Cost]]</f>
+        <v>5220</v>
       </c>
       <c r="J18" s="20" t="str">
         <f>Tabla1[[#This Row],[Quant]] &amp;" @" &amp;Tabla1[[#This Row],[Value]]</f>
@@ -2789,16 +2797,16 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
     <sortCondition ref="E2"/>
   </sortState>
   <conditionalFormatting sqref="E2:E5">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>